<commit_message>
Adicionando README ao projeto
</commit_message>
<xml_diff>
--- a/test_case_manual/test-cases-rubeus.xlsx
+++ b/test_case_manual/test-cases-rubeus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARQUIVOS BACKUP ARLEY\ESTUDOS\DESAFIOS - PROJETOS\QA\ps-rubeus\test_case_manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D68D97-764E-476A-98D0-EF91719EF21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B9362F-937F-4934-85AE-8C73EDF0744E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49067,7 +49067,7 @@
   <dimension ref="A1:X995"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>